<commit_message>
fix answers not counting correctly when written in upper case
</commit_message>
<xml_diff>
--- a/TeamProject/bin/Debug/Results.xlsx
+++ b/TeamProject/bin/Debug/Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>вввв</t>
   </si>
@@ -26,30 +26,30 @@
     <t>ффффффф</t>
   </si>
   <si>
+    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
+  </si>
+  <si>
+    <t>Buy Now!</t>
+  </si>
+  <si>
+    <t>mailto:support@e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Contact US</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
+  </si>
+  <si>
     <t>Spire.XLS for .NET</t>
   </si>
   <si>
-    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Contact US</t>
-  </si>
-  <si>
-    <t>mailto:support@e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Buy Now!</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
-  </si>
-  <si>
     <t>ввввв</t>
   </si>
   <si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>0/5</t>
+  </si>
+  <si>
+    <t>амогус</t>
+  </si>
+  <si>
+    <t>мид</t>
+  </si>
+  <si>
+    <t>боби</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -148,6 +157,20 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -212,7 +235,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="76">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="90">
       <alignment/>
       <protection/>
     </xf>
@@ -226,7 +249,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="76"/>
+    <cellStyle name="Hyperlink" xfId="90"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -619,7 +642,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -627,68 +650,82 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45048</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>22222</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="4">
         <v>45049</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.75">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="12.75">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>22222</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -737,42 +774,42 @@
   <sheetData>
     <row r="1" ht="12.75">
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="12.75">
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="12.75">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="12.75">
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="12.75">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" ht="12.75">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="12.75">
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more input checks
</commit_message>
<xml_diff>
--- a/TeamProject/bin/Debug/Results.xlsx
+++ b/TeamProject/bin/Debug/Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>вввв</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Группа:</t>
   </si>
   <si>
-    <t>Возраст</t>
-  </si>
-  <si>
     <t>Правильные ответы:</t>
   </si>
   <si>
@@ -117,6 +114,21 @@
   </si>
   <si>
     <t>к</t>
+  </si>
+  <si>
+    <t>Возраст:</t>
+  </si>
+  <si>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>ads</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -163,7 +175,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -187,6 +199,34 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,7 +361,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="146">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="174">
       <alignment/>
       <protection/>
     </xf>
@@ -335,7 +375,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="146"/>
+    <cellStyle name="Hyperlink" xfId="174"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -728,7 +768,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -742,35 +782,35 @@
         <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -778,13 +818,13 @@
     </row>
     <row r="4" spans="1:4" ht="12.75">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -792,41 +832,41 @@
     </row>
     <row r="5" spans="1:4" ht="12.75">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -834,40 +874,68 @@
     </row>
     <row r="8" spans="1:4" ht="12.75">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4">
-        <v>45048</v>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75">
       <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="12.75">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4">
+        <v>45048</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12.75">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>22222</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D11" s="4">
         <v>45049</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12.75">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" ht="12.75">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <v>22222</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>